<commit_message>
fixed some issues with part description and adjusted BOM
</commit_message>
<xml_diff>
--- a/fabrication/mdriver2_bom.xlsx
+++ b/fabrication/mdriver2_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvarx\src\mdriver2_hw\fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D234891-C5BD-48F9-B583-27C73E7CD885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4CE5A8-CC4C-4836-AD45-C2A748FD0407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FAD14C2B-BE5C-403D-83D8-866D5294208C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="193">
   <si>
     <t>Designator</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Resistor 0Ohm 0603</t>
   </si>
   <si>
-    <t>RC0402JR-070RL</t>
-  </si>
-  <si>
     <t>Resistor 10Ohm 0402</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>CRCW060356K0FKEA</t>
   </si>
   <si>
-    <t>Resistor 2.49Ohm 0402 1%</t>
-  </si>
-  <si>
     <t>CRCW04022K49FKED</t>
   </si>
   <si>
@@ -612,6 +606,15 @@
   </si>
   <si>
     <t>691709710302</t>
+  </si>
+  <si>
+    <t>RC0603JR-070RL</t>
+  </si>
+  <si>
+    <t>Resistor 2.49kOhm 0402 1%</t>
+  </si>
+  <si>
+    <t>CRGCQ0402F1M0</t>
   </si>
 </sst>
 </file>
@@ -989,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD89A116-113F-4D42-B877-244EA63A8DFF}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,13 +1010,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1279,7 +1282,7 @@
         <v>102</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1391,7 +1394,7 @@
         <v>113</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1402,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1416,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1430,10 +1433,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1444,10 +1447,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,10 +1475,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,10 +1503,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1514,10 +1517,10 @@
         <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1528,10 +1531,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,10 +1545,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1556,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1570,10 +1573,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1584,10 +1587,10 @@
         <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1598,10 +1601,10 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1612,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1626,10 +1629,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1640,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1654,10 +1657,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1668,10 +1671,10 @@
         <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1696,10 +1699,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1710,10 +1713,10 @@
         <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1724,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1738,10 +1741,10 @@
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,10 +1755,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1766,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1780,10 +1783,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1808,10 +1811,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1822,10 +1825,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1836,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1864,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1878,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1906,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1920,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed unused MLCCs from schematic and BOM
</commit_message>
<xml_diff>
--- a/fabrication/mdriver2_bom.xlsx
+++ b/fabrication/mdriver2_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvarx\src\mdriver2_hw\fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4CE5A8-CC4C-4836-AD45-C2A748FD0407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1F2AD-649A-403C-95B4-4F6E70C581CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FAD14C2B-BE5C-403D-83D8-866D5294208C}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>C1, C4, C7, C99, C131</t>
   </si>
   <si>
-    <t>C2, C3, C5, C15, C17, C18, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C56, C57, C58, C81, C82, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C100, C103, C104, C105, C107, C108, C109, C110, C111, C112, C113, C114, C115, C116, C117, C118, C119, C120, C121, C122, C123, C124, C125, C130, C132</t>
-  </si>
-  <si>
     <t>C6</t>
   </si>
   <si>
@@ -615,6 +612,9 @@
   </si>
   <si>
     <t>CRGCQ0402F1M0</t>
+  </si>
+  <si>
+    <t>C2, C3, C5, C15, C17, C21, C22, C23, C24, C25, C26, C29, C30, C31, C32, C33, C34, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C52, C53, C54, C56, C57, C58, C81, C82, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C100, C103, C104, C105, C107, C108, C109, C110, C111, C112, C113, C114, C115, C116, C117, C118, C119, C120, C121, C122, C123, C124, C125, C130, C132</t>
   </si>
 </sst>
 </file>
@@ -992,13 +992,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD89A116-113F-4D42-B877-244EA63A8DFF}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="133.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="78.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
@@ -1010,13 +1010,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1027,287 +1027,287 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B3" s="2">
         <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="1">
         <v>1433900000</v>
@@ -1315,27 +1315,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24" s="1">
         <v>74404042022</v>
@@ -1343,13 +1343,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="1">
         <v>74404032033</v>
@@ -1357,27 +1357,27 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="1">
         <v>61032021121</v>
@@ -1385,548 +1385,548 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
         <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2">
         <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2">
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2">
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2">
         <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2">
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2">
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2">
         <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2">
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2">
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="2">
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="2">
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2">
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="2">
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="2">
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="2">
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2">
         <v>1</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="2">
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="2">
         <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="2">
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="2">
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="2">
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue in parts description, footprint of RJ45 receptables, issues in BOM
</commit_message>
<xml_diff>
--- a/fabrication/mdriver2_bom.xlsx
+++ b/fabrication/mdriver2_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvarx\src\mdriver2_hw\fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1F2AD-649A-403C-95B4-4F6E70C581CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AE2C34-0A59-4FA4-BAAC-CAA5BDFDB30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FAD14C2B-BE5C-403D-83D8-866D5294208C}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{FAD14C2B-BE5C-403D-83D8-866D5294208C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,9 +329,6 @@
     <t>VLMS1300-GS08</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>MH2029-600Y</t>
   </si>
   <si>
@@ -615,6 +612,9 @@
   </si>
   <si>
     <t>C2, C3, C5, C15, C17, C21, C22, C23, C24, C25, C26, C29, C30, C31, C32, C33, C34, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C52, C53, C54, C56, C57, C58, C81, C82, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C100, C103, C104, C105, C107, C108, C109, C110, C111, C112, C113, C114, C115, C116, C117, C118, C119, C120, C121, C122, C123, C124, C125, C130, C132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	60 Ohms @ 100 MHz 1 Power, Signal Line Ferrite Bead 0805 (2012 Metric) 5A 20mOhm</t>
   </si>
 </sst>
 </file>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD89A116-113F-4D42-B877-244EA63A8DFF}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,13 +1010,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,7 +1035,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2">
         <v>80</v>
@@ -1251,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1265,10 +1265,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1279,10 +1279,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1293,10 +1293,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1307,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="1">
         <v>1433900000</v>
@@ -1321,10 +1321,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1">
         <v>74404042022</v>
@@ -1349,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="1">
         <v>74404032033</v>
@@ -1363,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1377,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D27" s="1">
         <v>61032021121</v>
@@ -1391,10 +1391,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1405,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1419,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1433,10 +1433,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1447,10 +1447,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1461,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1475,10 +1475,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1489,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1503,10 +1503,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1517,10 +1517,10 @@
         <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1531,10 +1531,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1545,10 +1545,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1559,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1573,10 +1573,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1587,10 +1587,10 @@
         <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1601,10 +1601,10 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1615,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1629,10 +1629,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1643,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1657,10 +1657,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1671,10 +1671,10 @@
         <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1685,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1699,10 +1699,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1713,10 +1713,10 @@
         <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1727,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1741,10 +1741,10 @@
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1755,10 +1755,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1769,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1783,10 +1783,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1797,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1811,10 +1811,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1825,10 +1825,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1839,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1853,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1867,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1881,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1895,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1909,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1923,13 +1923,14 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>